<commit_message>
28102025-1 bang bao gia
</commit_message>
<xml_diff>
--- a/database/exports/MAU-BANG-BAO-GIA.xlsx
+++ b/database/exports/MAU-BANG-BAO-GIA.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\var\www\adminlt\database\exports\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/4b1c315fe3860ed0/Van/02032021/Máy tính/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FE34085-B02C-45CA-BF16-E924D72FBB87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="36" documentId="8_{487313F0-1ADA-4B6F-8F49-44B9C41CC6DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1EA20DFB-415C-4D61-A1CA-3EE74FAEA0A0}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{AA2AB357-8B43-4900-A8BE-9AF4115D18D6}"/>
   </bookViews>
@@ -167,15 +167,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t>CÔNG TY TNHH INAFO VIỆT NAM</t>
-  </si>
-  <si>
-    <t>Địa chỉ: 240/127/26 Nguyễn Văn Luông, Phường 11, Quận 6, TP. Hồ Chí Minh</t>
-  </si>
-  <si>
-    <t>VPĐD: 23 Hát Giang, Phường 2, Quận Tân Bình, TP. Hồ Chí Minh</t>
   </si>
   <si>
     <t>Mã số thuế: 0314492345</t>
@@ -258,13 +252,16 @@
     <t>(Ký tên và đóng mộc công ty)</t>
   </si>
   <si>
-    <t>Kính gửi:</t>
+    <t>VPĐD: 36 Nguyễn Minh Hoàng, Phường Bảy Hiền, TP. Hồ Chí Minh</t>
   </si>
   <si>
-    <t xml:space="preserve"> QUÝ KHÁCH HÀNG</t>
+    <t>Địa chỉ: 240/127/26 Nguyễn Văn Luông, Phường Bình Phú, TP. Hồ Chí Minh</t>
   </si>
   <si>
-    <t>Tp.HCM, ngày 27 tháng 10 năm 2025</t>
+    <t xml:space="preserve">Kính gửi: </t>
+  </si>
+  <si>
+    <t>QUÝ KHÁCH HÀNG</t>
   </si>
 </sst>
 </file>
@@ -279,7 +276,7 @@
     <numFmt numFmtId="167" formatCode="_-* #,##0.00\ _₫_-;\-* #,##0.00\ _₫_-;_-* &quot;-&quot;??\ _₫_-;_-@_-"/>
     <numFmt numFmtId="168" formatCode="_-* #,##0\ _₫_-;\-* #,##0\ _₫_-;_-* &quot;-&quot;??\ _₫_-;_-@_-"/>
   </numFmts>
-  <fonts count="23">
+  <fonts count="22">
     <font>
       <sz val="14"/>
       <color theme="1"/>
@@ -414,13 +411,6 @@
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <name val="Calibri Light"/>
-      <family val="2"/>
-      <scheme val="major"/>
-    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -499,7 +489,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="3" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="4" applyFont="1" applyAlignment="1">
@@ -535,6 +525,9 @@
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="3" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="3" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="3" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -599,12 +592,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="3" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="14" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -620,8 +607,8 @@
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="14" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="9" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="15">
@@ -652,2296 +639,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:oneCellAnchor>
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>273745</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>40664</xdr:rowOff>
-    </xdr:from>
-    <xdr:ext cx="1563219" cy="852431"/>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C400CA01-1650-4E58-8337-9F5E93B8E3BE}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="273745" y="40664"/>
-          <a:ext cx="1563219" cy="852431"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:oneCellAnchor>
-  <xdr:oneCellAnchor>
-    <xdr:from>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:ext cx="114300" cy="76200"/>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="3" name="Text Box 1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3E0837FB-527B-4F96-97B0-83F7E909959F}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr txBox="1">
-          <a:spLocks noChangeArrowheads="1"/>
-        </xdr:cNvSpPr>
-      </xdr:nvSpPr>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="15097125" y="0"/>
-          <a:ext cx="114300" cy="76200"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:miter lim="800000"/>
-              <a:headEnd/>
-              <a:tailEnd/>
-            </a14:hiddenLine>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:oneCellAnchor>
-  <xdr:oneCellAnchor>
-    <xdr:from>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:ext cx="114300" cy="76200"/>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="4" name="Text Box 2">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5A26BE26-93FE-4607-A205-E092690B6D48}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr txBox="1">
-          <a:spLocks noChangeArrowheads="1"/>
-        </xdr:cNvSpPr>
-      </xdr:nvSpPr>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="15097125" y="0"/>
-          <a:ext cx="114300" cy="76200"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:miter lim="800000"/>
-              <a:headEnd/>
-              <a:tailEnd/>
-            </a14:hiddenLine>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:oneCellAnchor>
-  <xdr:oneCellAnchor>
-    <xdr:from>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:ext cx="114300" cy="76200"/>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="5" name="Text Box 1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FF1FA034-6FDB-47DF-ADA5-58FFD874B9C3}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr txBox="1">
-          <a:spLocks noChangeArrowheads="1"/>
-        </xdr:cNvSpPr>
-      </xdr:nvSpPr>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="15097125" y="0"/>
-          <a:ext cx="114300" cy="76200"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:miter lim="800000"/>
-              <a:headEnd/>
-              <a:tailEnd/>
-            </a14:hiddenLine>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:oneCellAnchor>
-  <xdr:oneCellAnchor>
-    <xdr:from>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:ext cx="114300" cy="76200"/>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="6" name="Text Box 2">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E79902F7-FD64-4022-8010-0DC425CBF590}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr txBox="1">
-          <a:spLocks noChangeArrowheads="1"/>
-        </xdr:cNvSpPr>
-      </xdr:nvSpPr>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="15097125" y="0"/>
-          <a:ext cx="114300" cy="76200"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:miter lim="800000"/>
-              <a:headEnd/>
-              <a:tailEnd/>
-            </a14:hiddenLine>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:oneCellAnchor>
-  <xdr:oneCellAnchor>
-    <xdr:from>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:ext cx="114300" cy="76200"/>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="7" name="Text Box 1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{81C8C24D-F990-4FAE-A684-083A01BFECE5}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr txBox="1">
-          <a:spLocks noChangeArrowheads="1"/>
-        </xdr:cNvSpPr>
-      </xdr:nvSpPr>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="15097125" y="0"/>
-          <a:ext cx="114300" cy="76200"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:miter lim="800000"/>
-              <a:headEnd/>
-              <a:tailEnd/>
-            </a14:hiddenLine>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:oneCellAnchor>
-  <xdr:oneCellAnchor>
-    <xdr:from>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:ext cx="114300" cy="76200"/>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="8" name="Text Box 2">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{947E6DCF-60D5-4F34-9765-956340D842CA}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr txBox="1">
-          <a:spLocks noChangeArrowheads="1"/>
-        </xdr:cNvSpPr>
-      </xdr:nvSpPr>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="15097125" y="0"/>
-          <a:ext cx="114300" cy="76200"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:miter lim="800000"/>
-              <a:headEnd/>
-              <a:tailEnd/>
-            </a14:hiddenLine>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:oneCellAnchor>
-  <xdr:oneCellAnchor>
-    <xdr:from>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:ext cx="114300" cy="76200"/>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="9" name="Text Box 1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A5B9F280-0B64-4D52-89AE-0B24F98955FA}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr txBox="1">
-          <a:spLocks noChangeArrowheads="1"/>
-        </xdr:cNvSpPr>
-      </xdr:nvSpPr>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="15097125" y="0"/>
-          <a:ext cx="114300" cy="76200"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:miter lim="800000"/>
-              <a:headEnd/>
-              <a:tailEnd/>
-            </a14:hiddenLine>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:oneCellAnchor>
-  <xdr:oneCellAnchor>
-    <xdr:from>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:ext cx="114300" cy="76200"/>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="10" name="Text Box 2">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0B8EAB74-ECB3-4D8C-A79B-14E41C37EA32}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr txBox="1">
-          <a:spLocks noChangeArrowheads="1"/>
-        </xdr:cNvSpPr>
-      </xdr:nvSpPr>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="15097125" y="0"/>
-          <a:ext cx="114300" cy="76200"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:miter lim="800000"/>
-              <a:headEnd/>
-              <a:tailEnd/>
-            </a14:hiddenLine>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:oneCellAnchor>
-  <xdr:oneCellAnchor>
-    <xdr:from>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:ext cx="114300" cy="76200"/>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="11" name="Text Box 1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{86F6F86C-4DD0-4F0D-80AB-D89B3EA09E12}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr txBox="1">
-          <a:spLocks noChangeArrowheads="1"/>
-        </xdr:cNvSpPr>
-      </xdr:nvSpPr>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="15097125" y="0"/>
-          <a:ext cx="114300" cy="76200"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:miter lim="800000"/>
-              <a:headEnd/>
-              <a:tailEnd/>
-            </a14:hiddenLine>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:oneCellAnchor>
-  <xdr:oneCellAnchor>
-    <xdr:from>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:ext cx="114300" cy="76200"/>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="12" name="Text Box 2">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8A77D0FC-0A14-417C-93FF-F4B7888BBC9B}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr txBox="1">
-          <a:spLocks noChangeArrowheads="1"/>
-        </xdr:cNvSpPr>
-      </xdr:nvSpPr>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="15097125" y="0"/>
-          <a:ext cx="114300" cy="76200"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:miter lim="800000"/>
-              <a:headEnd/>
-              <a:tailEnd/>
-            </a14:hiddenLine>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:oneCellAnchor>
-  <xdr:oneCellAnchor>
-    <xdr:from>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:ext cx="114300" cy="76200"/>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="13" name="Text Box 1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BA4C0F9C-87C2-4790-AEDB-905369136DB2}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr txBox="1">
-          <a:spLocks noChangeArrowheads="1"/>
-        </xdr:cNvSpPr>
-      </xdr:nvSpPr>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="15097125" y="0"/>
-          <a:ext cx="114300" cy="76200"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:miter lim="800000"/>
-              <a:headEnd/>
-              <a:tailEnd/>
-            </a14:hiddenLine>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:oneCellAnchor>
-  <xdr:oneCellAnchor>
-    <xdr:from>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:ext cx="114300" cy="76200"/>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="14" name="Text Box 2">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8CB13BE2-E7DE-46BE-A922-6D87C6322EEB}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr txBox="1">
-          <a:spLocks noChangeArrowheads="1"/>
-        </xdr:cNvSpPr>
-      </xdr:nvSpPr>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="15097125" y="0"/>
-          <a:ext cx="114300" cy="76200"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:miter lim="800000"/>
-              <a:headEnd/>
-              <a:tailEnd/>
-            </a14:hiddenLine>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:oneCellAnchor>
-  <xdr:oneCellAnchor>
-    <xdr:from>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:ext cx="114300" cy="76200"/>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="15" name="Text Box 1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{07799405-83E1-4B87-9977-80007934B562}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr txBox="1">
-          <a:spLocks noChangeArrowheads="1"/>
-        </xdr:cNvSpPr>
-      </xdr:nvSpPr>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="15097125" y="0"/>
-          <a:ext cx="114300" cy="76200"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:miter lim="800000"/>
-              <a:headEnd/>
-              <a:tailEnd/>
-            </a14:hiddenLine>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:oneCellAnchor>
-  <xdr:oneCellAnchor>
-    <xdr:from>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:ext cx="114300" cy="76200"/>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="16" name="Text Box 2">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7165E822-7C8A-4534-B552-9C848E759C3C}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr txBox="1">
-          <a:spLocks noChangeArrowheads="1"/>
-        </xdr:cNvSpPr>
-      </xdr:nvSpPr>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="15097125" y="0"/>
-          <a:ext cx="114300" cy="76200"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:miter lim="800000"/>
-              <a:headEnd/>
-              <a:tailEnd/>
-            </a14:hiddenLine>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:oneCellAnchor>
-  <xdr:oneCellAnchor>
-    <xdr:from>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:ext cx="114300" cy="76200"/>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="17" name="Text Box 1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A503F360-CCEA-4364-BBE7-1C49157A1688}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr txBox="1">
-          <a:spLocks noChangeArrowheads="1"/>
-        </xdr:cNvSpPr>
-      </xdr:nvSpPr>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="15097125" y="0"/>
-          <a:ext cx="114300" cy="76200"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:miter lim="800000"/>
-              <a:headEnd/>
-              <a:tailEnd/>
-            </a14:hiddenLine>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:oneCellAnchor>
-  <xdr:oneCellAnchor>
-    <xdr:from>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:ext cx="114300" cy="76200"/>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="18" name="Text Box 2">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9EBE310B-B79D-44D6-BABB-6A78BA66160A}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr txBox="1">
-          <a:spLocks noChangeArrowheads="1"/>
-        </xdr:cNvSpPr>
-      </xdr:nvSpPr>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="15097125" y="0"/>
-          <a:ext cx="114300" cy="76200"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:miter lim="800000"/>
-              <a:headEnd/>
-              <a:tailEnd/>
-            </a14:hiddenLine>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:oneCellAnchor>
-  <xdr:oneCellAnchor>
-    <xdr:from>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:ext cx="114300" cy="76200"/>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="19" name="Text Box 1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EF0DEF29-954A-47C0-BD72-431B66C0FFAC}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr txBox="1">
-          <a:spLocks noChangeArrowheads="1"/>
-        </xdr:cNvSpPr>
-      </xdr:nvSpPr>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="15097125" y="0"/>
-          <a:ext cx="114300" cy="76200"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:miter lim="800000"/>
-              <a:headEnd/>
-              <a:tailEnd/>
-            </a14:hiddenLine>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:oneCellAnchor>
-  <xdr:oneCellAnchor>
-    <xdr:from>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:ext cx="114300" cy="76200"/>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="20" name="Text Box 2">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0222E49E-1F9A-4890-AA59-0B9AD9C28323}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr txBox="1">
-          <a:spLocks noChangeArrowheads="1"/>
-        </xdr:cNvSpPr>
-      </xdr:nvSpPr>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="15097125" y="0"/>
-          <a:ext cx="114300" cy="76200"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:miter lim="800000"/>
-              <a:headEnd/>
-              <a:tailEnd/>
-            </a14:hiddenLine>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:oneCellAnchor>
-  <xdr:oneCellAnchor>
-    <xdr:from>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:ext cx="114300" cy="76200"/>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="21" name="Text Box 1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B2A52D6D-E6F6-4E44-85E2-827E40EFCD50}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr txBox="1">
-          <a:spLocks noChangeArrowheads="1"/>
-        </xdr:cNvSpPr>
-      </xdr:nvSpPr>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="15097125" y="0"/>
-          <a:ext cx="114300" cy="76200"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:miter lim="800000"/>
-              <a:headEnd/>
-              <a:tailEnd/>
-            </a14:hiddenLine>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:oneCellAnchor>
-  <xdr:oneCellAnchor>
-    <xdr:from>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:ext cx="114300" cy="76200"/>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="22" name="Text Box 2">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{012562FD-66ED-4355-9DC7-5384BC44AE3D}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr txBox="1">
-          <a:spLocks noChangeArrowheads="1"/>
-        </xdr:cNvSpPr>
-      </xdr:nvSpPr>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="15097125" y="0"/>
-          <a:ext cx="114300" cy="76200"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:miter lim="800000"/>
-              <a:headEnd/>
-              <a:tailEnd/>
-            </a14:hiddenLine>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:oneCellAnchor>
-  <xdr:oneCellAnchor>
-    <xdr:from>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:ext cx="114300" cy="76200"/>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="23" name="Text Box 1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0FA54BC6-82B8-43B7-B3D2-29BC32D2B6FF}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr txBox="1">
-          <a:spLocks noChangeArrowheads="1"/>
-        </xdr:cNvSpPr>
-      </xdr:nvSpPr>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="15097125" y="0"/>
-          <a:ext cx="114300" cy="76200"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:miter lim="800000"/>
-              <a:headEnd/>
-              <a:tailEnd/>
-            </a14:hiddenLine>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:oneCellAnchor>
-  <xdr:oneCellAnchor>
-    <xdr:from>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:ext cx="114300" cy="76200"/>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="24" name="Text Box 2">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D36194B3-644A-43FD-89AC-DB6071981620}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr txBox="1">
-          <a:spLocks noChangeArrowheads="1"/>
-        </xdr:cNvSpPr>
-      </xdr:nvSpPr>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="15097125" y="0"/>
-          <a:ext cx="114300" cy="76200"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:miter lim="800000"/>
-              <a:headEnd/>
-              <a:tailEnd/>
-            </a14:hiddenLine>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:oneCellAnchor>
-  <xdr:oneCellAnchor>
-    <xdr:from>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:ext cx="114300" cy="76200"/>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="25" name="Text Box 1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{91026982-7B91-4CCD-9257-A2124B078636}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr txBox="1">
-          <a:spLocks noChangeArrowheads="1"/>
-        </xdr:cNvSpPr>
-      </xdr:nvSpPr>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="15097125" y="0"/>
-          <a:ext cx="114300" cy="76200"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:miter lim="800000"/>
-              <a:headEnd/>
-              <a:tailEnd/>
-            </a14:hiddenLine>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:oneCellAnchor>
-  <xdr:oneCellAnchor>
-    <xdr:from>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:ext cx="114300" cy="76200"/>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="26" name="Text Box 2">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{796C32AD-2BCA-4D65-849E-2C1827AB8C33}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr txBox="1">
-          <a:spLocks noChangeArrowheads="1"/>
-        </xdr:cNvSpPr>
-      </xdr:nvSpPr>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="15097125" y="0"/>
-          <a:ext cx="114300" cy="76200"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:miter lim="800000"/>
-              <a:headEnd/>
-              <a:tailEnd/>
-            </a14:hiddenLine>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:oneCellAnchor>
-  <xdr:oneCellAnchor>
-    <xdr:from>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:ext cx="114300" cy="76200"/>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="27" name="Text Box 1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B702B0C6-9ED5-4CB6-B48D-32C99FF5CEB8}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr txBox="1">
-          <a:spLocks noChangeArrowheads="1"/>
-        </xdr:cNvSpPr>
-      </xdr:nvSpPr>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="15097125" y="0"/>
-          <a:ext cx="114300" cy="76200"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:miter lim="800000"/>
-              <a:headEnd/>
-              <a:tailEnd/>
-            </a14:hiddenLine>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:oneCellAnchor>
-  <xdr:oneCellAnchor>
-    <xdr:from>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:ext cx="114300" cy="76200"/>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="28" name="Text Box 2">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{04A22686-F1AD-4C48-999E-99519742F526}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr txBox="1">
-          <a:spLocks noChangeArrowheads="1"/>
-        </xdr:cNvSpPr>
-      </xdr:nvSpPr>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="15097125" y="0"/>
-          <a:ext cx="114300" cy="76200"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:miter lim="800000"/>
-              <a:headEnd/>
-              <a:tailEnd/>
-            </a14:hiddenLine>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:oneCellAnchor>
-  <xdr:oneCellAnchor>
-    <xdr:from>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:ext cx="114300" cy="76200"/>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="29" name="Text Box 1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2E7D47DE-437C-42F6-BF43-C294DB63C2DB}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr txBox="1">
-          <a:spLocks noChangeArrowheads="1"/>
-        </xdr:cNvSpPr>
-      </xdr:nvSpPr>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="15097125" y="0"/>
-          <a:ext cx="114300" cy="76200"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:miter lim="800000"/>
-              <a:headEnd/>
-              <a:tailEnd/>
-            </a14:hiddenLine>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:oneCellAnchor>
-  <xdr:oneCellAnchor>
-    <xdr:from>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:ext cx="114300" cy="76200"/>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="30" name="Text Box 2">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{59F6E764-5178-4934-8CDD-933275874D4F}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr txBox="1">
-          <a:spLocks noChangeArrowheads="1"/>
-        </xdr:cNvSpPr>
-      </xdr:nvSpPr>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="15097125" y="0"/>
-          <a:ext cx="114300" cy="76200"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:miter lim="800000"/>
-              <a:headEnd/>
-              <a:tailEnd/>
-            </a14:hiddenLine>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:oneCellAnchor>
-  <xdr:oneCellAnchor>
-    <xdr:from>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:ext cx="114300" cy="76200"/>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="31" name="Text Box 1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3E0F0994-0E72-436C-8B38-A3FDF78322F8}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr txBox="1">
-          <a:spLocks noChangeArrowheads="1"/>
-        </xdr:cNvSpPr>
-      </xdr:nvSpPr>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="15097125" y="0"/>
-          <a:ext cx="114300" cy="76200"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:miter lim="800000"/>
-              <a:headEnd/>
-              <a:tailEnd/>
-            </a14:hiddenLine>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:oneCellAnchor>
-  <xdr:oneCellAnchor>
-    <xdr:from>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:ext cx="114300" cy="76200"/>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="32" name="Text Box 2">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4D87D8BD-27CC-46F2-A51C-D89BDBE8BD4E}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr txBox="1">
-          <a:spLocks noChangeArrowheads="1"/>
-        </xdr:cNvSpPr>
-      </xdr:nvSpPr>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="15097125" y="0"/>
-          <a:ext cx="114300" cy="76200"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:miter lim="800000"/>
-              <a:headEnd/>
-              <a:tailEnd/>
-            </a14:hiddenLine>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:oneCellAnchor>
-  <xdr:oneCellAnchor>
-    <xdr:from>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:ext cx="114300" cy="76200"/>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="33" name="Text Box 1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5AF1DF1F-4839-4B2A-85A1-92B37A53E387}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr txBox="1">
-          <a:spLocks noChangeArrowheads="1"/>
-        </xdr:cNvSpPr>
-      </xdr:nvSpPr>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="15097125" y="0"/>
-          <a:ext cx="114300" cy="76200"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:miter lim="800000"/>
-              <a:headEnd/>
-              <a:tailEnd/>
-            </a14:hiddenLine>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:oneCellAnchor>
-  <xdr:oneCellAnchor>
-    <xdr:from>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:ext cx="114300" cy="76200"/>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="34" name="Text Box 2">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5C6014EB-7F31-4957-A273-6ABF0EC4CCE5}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr txBox="1">
-          <a:spLocks noChangeArrowheads="1"/>
-        </xdr:cNvSpPr>
-      </xdr:nvSpPr>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="15097125" y="0"/>
-          <a:ext cx="114300" cy="76200"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:miter lim="800000"/>
-              <a:headEnd/>
-              <a:tailEnd/>
-            </a14:hiddenLine>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:oneCellAnchor>
-  <xdr:oneCellAnchor>
-    <xdr:from>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:ext cx="114300" cy="76200"/>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="35" name="Text Box 1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{789AE133-0633-48FC-8088-A2549D568F23}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr txBox="1">
-          <a:spLocks noChangeArrowheads="1"/>
-        </xdr:cNvSpPr>
-      </xdr:nvSpPr>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="15097125" y="0"/>
-          <a:ext cx="114300" cy="76200"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:miter lim="800000"/>
-              <a:headEnd/>
-              <a:tailEnd/>
-            </a14:hiddenLine>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:oneCellAnchor>
-  <xdr:oneCellAnchor>
-    <xdr:from>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:ext cx="114300" cy="76200"/>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="36" name="Text Box 2">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AA399B71-7164-4075-BEBF-19774B26CC1D}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr txBox="1">
-          <a:spLocks noChangeArrowheads="1"/>
-        </xdr:cNvSpPr>
-      </xdr:nvSpPr>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="15097125" y="0"/>
-          <a:ext cx="114300" cy="76200"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:miter lim="800000"/>
-              <a:headEnd/>
-              <a:tailEnd/>
-            </a14:hiddenLine>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:oneCellAnchor>
-  <xdr:oneCellAnchor>
-    <xdr:from>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:ext cx="114300" cy="76200"/>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="37" name="Text Box 1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{35749D77-9123-4DE9-801C-2386C8E02833}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr txBox="1">
-          <a:spLocks noChangeArrowheads="1"/>
-        </xdr:cNvSpPr>
-      </xdr:nvSpPr>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="15097125" y="0"/>
-          <a:ext cx="114300" cy="76200"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:miter lim="800000"/>
-              <a:headEnd/>
-              <a:tailEnd/>
-            </a14:hiddenLine>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:oneCellAnchor>
-  <xdr:oneCellAnchor>
-    <xdr:from>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:ext cx="114300" cy="76200"/>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="38" name="Text Box 2">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{ADDFC99C-1DF8-4C1D-8770-66436CFB8841}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr txBox="1">
-          <a:spLocks noChangeArrowheads="1"/>
-        </xdr:cNvSpPr>
-      </xdr:nvSpPr>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="15097125" y="0"/>
-          <a:ext cx="114300" cy="76200"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:miter lim="800000"/>
-              <a:headEnd/>
-              <a:tailEnd/>
-            </a14:hiddenLine>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:oneCellAnchor>
-  <xdr:oneCellAnchor>
-    <xdr:from>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:ext cx="114300" cy="76200"/>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="39" name="Text Box 1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BDC74ED7-BA77-4871-AC7B-8DD7D7279451}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr txBox="1">
-          <a:spLocks noChangeArrowheads="1"/>
-        </xdr:cNvSpPr>
-      </xdr:nvSpPr>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="15097125" y="0"/>
-          <a:ext cx="114300" cy="76200"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:miter lim="800000"/>
-              <a:headEnd/>
-              <a:tailEnd/>
-            </a14:hiddenLine>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:oneCellAnchor>
-  <xdr:oneCellAnchor>
-    <xdr:from>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:ext cx="114300" cy="76200"/>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="40" name="Text Box 2">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BB1816F1-CB7A-46AF-80C9-99967F82E0F2}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr txBox="1">
-          <a:spLocks noChangeArrowheads="1"/>
-        </xdr:cNvSpPr>
-      </xdr:nvSpPr>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="15097125" y="0"/>
-          <a:ext cx="114300" cy="76200"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:miter lim="800000"/>
-              <a:headEnd/>
-              <a:tailEnd/>
-            </a14:hiddenLine>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:oneCellAnchor>
-  <xdr:oneCellAnchor>
-    <xdr:from>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:ext cx="114300" cy="76200"/>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="41" name="Text Box 1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E76ECFC7-491D-4212-8D83-6BDA8FBCA967}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr txBox="1">
-          <a:spLocks noChangeArrowheads="1"/>
-        </xdr:cNvSpPr>
-      </xdr:nvSpPr>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="15097125" y="0"/>
-          <a:ext cx="114300" cy="76200"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:miter lim="800000"/>
-              <a:headEnd/>
-              <a:tailEnd/>
-            </a14:hiddenLine>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:oneCellAnchor>
-  <xdr:oneCellAnchor>
-    <xdr:from>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:ext cx="114300" cy="76200"/>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="42" name="Text Box 2">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{70F5D49C-7C7F-4263-A7A3-9AD389193D53}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr txBox="1">
-          <a:spLocks noChangeArrowheads="1"/>
-        </xdr:cNvSpPr>
-      </xdr:nvSpPr>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="15097125" y="0"/>
-          <a:ext cx="114300" cy="76200"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:miter lim="800000"/>
-              <a:headEnd/>
-              <a:tailEnd/>
-            </a14:hiddenLine>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:oneCellAnchor>
-</xdr:wsDr>
 </file>
 
 <file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -31414,10 +29111,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8326482F-38D0-4A78-9C12-23F885EAB698}">
-  <dimension ref="A1:N51"/>
+  <dimension ref="A1:N50"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="L12" sqref="L12:N12"/>
+      <selection activeCell="L19" sqref="L19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.36328125" defaultRowHeight="16.8"/>
@@ -31425,7 +29122,7 @@
     <col min="1" max="1" width="5.1796875" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.81640625" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.81640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.36328125" style="33" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.36328125" style="34" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.453125" style="1" customWidth="1"/>
     <col min="6" max="6" width="19.08984375" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="17.54296875" style="1" bestFit="1" customWidth="1"/>
@@ -33031,321 +30728,301 @@
     </row>
     <row r="2" spans="1:14">
       <c r="D2" s="5" t="s">
-        <v>1</v>
+        <v>22</v>
       </c>
       <c r="N2" s="6"/>
     </row>
     <row r="3" spans="1:14">
       <c r="D3" s="5" t="s">
-        <v>2</v>
+        <v>21</v>
       </c>
       <c r="N3" s="6"/>
     </row>
     <row r="4" spans="1:14">
       <c r="D4" s="5" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="N4" s="4"/>
     </row>
     <row r="5" spans="1:14">
       <c r="D5" s="5" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
-      <c r="G5" s="40"/>
-      <c r="H5" s="40"/>
-      <c r="I5" s="40"/>
-      <c r="J5" s="40"/>
-      <c r="K5" s="40"/>
-      <c r="L5" s="40"/>
-      <c r="M5" s="40"/>
+      <c r="G5" s="39"/>
+      <c r="H5" s="39"/>
+      <c r="I5" s="39"/>
+      <c r="J5" s="39"/>
+      <c r="K5" s="39"/>
+      <c r="L5" s="39"/>
+      <c r="M5" s="39"/>
       <c r="N5" s="6"/>
     </row>
     <row r="6" spans="1:14" ht="46.5" customHeight="1">
-      <c r="A6" s="41" t="s">
-        <v>5</v>
+      <c r="A6" s="40" t="s">
+        <v>3</v>
       </c>
-      <c r="B6" s="41"/>
-      <c r="C6" s="41"/>
-      <c r="D6" s="41"/>
-      <c r="E6" s="41"/>
-      <c r="F6" s="41"/>
-      <c r="G6" s="41"/>
-      <c r="H6" s="41"/>
-      <c r="I6" s="41"/>
-      <c r="J6" s="41"/>
-      <c r="K6" s="41"/>
-      <c r="L6" s="41"/>
-      <c r="M6" s="41"/>
-      <c r="N6" s="41"/>
+      <c r="B6" s="40"/>
+      <c r="C6" s="40"/>
+      <c r="D6" s="40"/>
+      <c r="E6" s="40"/>
+      <c r="F6" s="40"/>
+      <c r="G6" s="40"/>
+      <c r="H6" s="40"/>
+      <c r="I6" s="40"/>
+      <c r="J6" s="40"/>
+      <c r="K6" s="40"/>
+      <c r="L6" s="40"/>
+      <c r="M6" s="40"/>
+      <c r="N6" s="40"/>
     </row>
     <row r="7" spans="1:14" s="7" customFormat="1" ht="27.75" customHeight="1">
-      <c r="A7" s="37" t="s">
+      <c r="A7" s="43" t="s">
         <v>23</v>
       </c>
-      <c r="B7" s="37"/>
-      <c r="C7" s="37" t="s">
+      <c r="B7" s="43"/>
+      <c r="C7" s="43" t="s">
         <v>24</v>
       </c>
-      <c r="D7" s="37"/>
-      <c r="E7" s="37"/>
-      <c r="F7" s="37"/>
-      <c r="G7" s="37"/>
-      <c r="H7" s="37"/>
-      <c r="I7" s="37"/>
-      <c r="J7" s="37"/>
-      <c r="K7" s="37"/>
-      <c r="L7" s="37"/>
-      <c r="M7" s="37"/>
-      <c r="N7" s="37"/>
+      <c r="D7" s="43"/>
+      <c r="E7" s="43"/>
+      <c r="F7" s="43"/>
+      <c r="G7" s="43"/>
+      <c r="H7" s="43"/>
+      <c r="I7" s="43"/>
+      <c r="J7" s="43"/>
+      <c r="K7" s="43"/>
+      <c r="L7" s="43"/>
+      <c r="M7" s="43"/>
+      <c r="N7" s="43"/>
     </row>
     <row r="8" spans="1:14" ht="25.5" customHeight="1">
-      <c r="A8" s="42" t="s">
-        <v>6</v>
+      <c r="A8" s="41" t="s">
+        <v>4</v>
       </c>
-      <c r="B8" s="42"/>
-      <c r="C8" s="42"/>
-      <c r="D8" s="42"/>
-      <c r="E8" s="42"/>
-      <c r="F8" s="42"/>
-      <c r="G8" s="42"/>
-      <c r="H8" s="42"/>
-      <c r="I8" s="42"/>
-      <c r="J8" s="42"/>
-      <c r="K8" s="42"/>
-      <c r="L8" s="42"/>
-      <c r="M8" s="42"/>
-      <c r="N8" s="42"/>
+      <c r="B8" s="41"/>
+      <c r="C8" s="41"/>
+      <c r="D8" s="41"/>
+      <c r="E8" s="41"/>
+      <c r="F8" s="41"/>
+      <c r="G8" s="41"/>
+      <c r="H8" s="41"/>
+      <c r="I8" s="41"/>
+      <c r="J8" s="41"/>
+      <c r="K8" s="41"/>
+      <c r="L8" s="41"/>
+      <c r="M8" s="41"/>
+      <c r="N8" s="41"/>
     </row>
     <row r="9" spans="1:14" ht="101.25" customHeight="1">
       <c r="A9" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="B9" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="8" t="s">
+      <c r="D9" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="8" t="s">
+      <c r="E9" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="D9" s="8" t="s">
+      <c r="F9" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="E9" s="8" t="s">
+      <c r="G9" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="F9" s="8" t="s">
+      <c r="H9" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="G9" s="8" t="s">
+      <c r="I9" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="H9" s="8" t="s">
+      <c r="J9" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="I9" s="8" t="s">
+      <c r="K9" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="J9" s="8" t="s">
+      <c r="L9" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="K9" s="9" t="s">
+      <c r="M9" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="L9" s="10" t="s">
+      <c r="N9" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="M9" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="N9" s="8" t="s">
-        <v>20</v>
-      </c>
     </row>
-    <row r="10" spans="1:14" s="21" customFormat="1" ht="14.4">
+    <row r="10" spans="1:14" s="22" customFormat="1" ht="14.4">
       <c r="A10" s="11"/>
       <c r="B10" s="12"/>
       <c r="C10" s="13"/>
-      <c r="D10" s="38"/>
+      <c r="D10" s="14"/>
       <c r="E10" s="11"/>
-      <c r="F10" s="14"/>
-      <c r="G10" s="15"/>
-      <c r="H10" s="16"/>
-      <c r="I10" s="16"/>
-      <c r="J10" s="17"/>
-      <c r="K10" s="18"/>
-      <c r="L10" s="19"/>
-      <c r="M10" s="20"/>
-      <c r="N10" s="20"/>
+      <c r="F10" s="15"/>
+      <c r="G10" s="16"/>
+      <c r="H10" s="17"/>
+      <c r="I10" s="17"/>
+      <c r="J10" s="18"/>
+      <c r="K10" s="19"/>
+      <c r="L10" s="20"/>
+      <c r="M10" s="21"/>
+      <c r="N10" s="21"/>
     </row>
-    <row r="11" spans="1:14" s="21" customFormat="1">
-      <c r="A11" s="22"/>
-      <c r="B11" s="23"/>
-      <c r="C11" s="24"/>
-      <c r="D11" s="25"/>
-      <c r="E11" s="22"/>
-      <c r="F11" s="26"/>
-      <c r="G11" s="27"/>
-      <c r="H11" s="27"/>
-      <c r="I11" s="27"/>
-      <c r="J11" s="28"/>
-      <c r="K11" s="29"/>
-      <c r="L11" s="30"/>
-      <c r="M11" s="31"/>
-      <c r="N11" s="31"/>
+    <row r="11" spans="1:14" s="22" customFormat="1">
+      <c r="A11" s="23"/>
+      <c r="B11" s="24"/>
+      <c r="C11" s="25"/>
+      <c r="D11" s="26"/>
+      <c r="E11" s="23"/>
+      <c r="F11" s="27"/>
+      <c r="G11" s="28"/>
+      <c r="H11" s="28"/>
+      <c r="I11" s="28"/>
+      <c r="J11" s="29"/>
+      <c r="K11" s="30"/>
+      <c r="L11" s="31"/>
+      <c r="M11" s="32"/>
+      <c r="N11" s="32"/>
     </row>
-    <row r="12" spans="1:14" s="21" customFormat="1" ht="28.8" customHeight="1">
-      <c r="A12" s="22"/>
-      <c r="B12" s="23"/>
-      <c r="C12" s="24"/>
-      <c r="D12" s="25"/>
-      <c r="E12" s="22"/>
-      <c r="F12" s="26"/>
-      <c r="G12" s="27"/>
-      <c r="H12" s="27"/>
-      <c r="I12" s="27"/>
-      <c r="J12" s="28"/>
-      <c r="K12" s="29"/>
-      <c r="L12" s="44" t="s">
-        <v>25</v>
+    <row r="12" spans="1:14">
+      <c r="B12" s="33"/>
+      <c r="J12" s="42" t="s">
+        <v>19</v>
       </c>
-      <c r="M12" s="44"/>
-      <c r="N12" s="44"/>
+      <c r="K12" s="42"/>
+      <c r="L12" s="42"/>
+      <c r="M12" s="42"/>
+      <c r="N12" s="42"/>
     </row>
     <row r="13" spans="1:14">
-      <c r="B13" s="32"/>
-      <c r="J13" s="43" t="s">
-        <v>21</v>
+      <c r="B13" s="33"/>
+      <c r="D13" s="37"/>
+      <c r="J13" s="38" t="s">
+        <v>20</v>
       </c>
-      <c r="K13" s="43"/>
-      <c r="L13" s="43"/>
-      <c r="M13" s="43"/>
-      <c r="N13" s="43"/>
+      <c r="K13" s="38"/>
+      <c r="L13" s="38"/>
+      <c r="M13" s="38"/>
+      <c r="N13" s="38"/>
     </row>
     <row r="14" spans="1:14">
-      <c r="B14" s="32"/>
-      <c r="D14" s="36"/>
-      <c r="J14" s="39" t="s">
-        <v>22</v>
-      </c>
-      <c r="K14" s="39"/>
-      <c r="L14" s="39"/>
-      <c r="M14" s="39"/>
-      <c r="N14" s="39"/>
+      <c r="B14" s="33"/>
     </row>
     <row r="15" spans="1:14">
-      <c r="B15" s="32"/>
+      <c r="B15" s="33"/>
     </row>
     <row r="16" spans="1:14">
-      <c r="B16" s="32"/>
+      <c r="B16" s="33"/>
+      <c r="K16" s="35"/>
     </row>
-    <row r="17" spans="2:11">
-      <c r="B17" s="32"/>
-      <c r="K17" s="34"/>
+    <row r="17" spans="2:2">
+      <c r="B17" s="33"/>
     </row>
-    <row r="18" spans="2:11">
-      <c r="B18" s="32"/>
+    <row r="18" spans="2:2">
+      <c r="B18" s="33"/>
     </row>
-    <row r="19" spans="2:11">
-      <c r="B19" s="32"/>
+    <row r="19" spans="2:2">
+      <c r="B19" s="33"/>
     </row>
-    <row r="20" spans="2:11">
-      <c r="B20" s="32"/>
+    <row r="20" spans="2:2">
+      <c r="B20" s="33"/>
     </row>
-    <row r="21" spans="2:11">
-      <c r="B21" s="32"/>
+    <row r="21" spans="2:2">
+      <c r="B21" s="33"/>
     </row>
-    <row r="22" spans="2:11">
-      <c r="B22" s="32"/>
+    <row r="22" spans="2:2">
+      <c r="B22" s="33"/>
     </row>
-    <row r="23" spans="2:11">
-      <c r="B23" s="32"/>
+    <row r="23" spans="2:2">
+      <c r="B23" s="33"/>
     </row>
-    <row r="24" spans="2:11">
-      <c r="B24" s="32"/>
+    <row r="24" spans="2:2">
+      <c r="B24" s="33"/>
     </row>
-    <row r="25" spans="2:11">
-      <c r="B25" s="32"/>
+    <row r="25" spans="2:2">
+      <c r="B25" s="33"/>
     </row>
-    <row r="26" spans="2:11">
-      <c r="B26" s="32"/>
+    <row r="26" spans="2:2">
+      <c r="B26" s="33"/>
     </row>
-    <row r="27" spans="2:11">
-      <c r="B27" s="32"/>
+    <row r="27" spans="2:2">
+      <c r="B27" s="33"/>
     </row>
-    <row r="28" spans="2:11">
-      <c r="B28" s="32"/>
+    <row r="28" spans="2:2">
+      <c r="B28" s="33"/>
     </row>
-    <row r="29" spans="2:11">
-      <c r="B29" s="32"/>
+    <row r="29" spans="2:2">
+      <c r="B29" s="33"/>
     </row>
-    <row r="30" spans="2:11">
-      <c r="B30" s="32"/>
+    <row r="30" spans="2:2">
+      <c r="B30" s="33"/>
     </row>
-    <row r="31" spans="2:11">
-      <c r="B31" s="32"/>
+    <row r="31" spans="2:2">
+      <c r="B31" s="33"/>
     </row>
-    <row r="32" spans="2:11">
-      <c r="B32" s="32"/>
+    <row r="32" spans="2:2">
+      <c r="B32" s="33"/>
     </row>
     <row r="33" spans="2:2">
-      <c r="B33" s="32"/>
+      <c r="B33" s="33"/>
     </row>
     <row r="34" spans="2:2">
-      <c r="B34" s="32"/>
+      <c r="B34" s="33"/>
     </row>
     <row r="35" spans="2:2">
-      <c r="B35" s="32"/>
+      <c r="B35" s="33"/>
     </row>
     <row r="36" spans="2:2">
-      <c r="B36" s="32"/>
+      <c r="B36" s="33"/>
     </row>
     <row r="37" spans="2:2">
-      <c r="B37" s="32"/>
+      <c r="B37" s="33"/>
     </row>
     <row r="38" spans="2:2">
-      <c r="B38" s="32"/>
+      <c r="B38" s="33"/>
     </row>
     <row r="39" spans="2:2">
-      <c r="B39" s="32"/>
+      <c r="B39" s="33"/>
     </row>
     <row r="40" spans="2:2">
-      <c r="B40" s="32"/>
+      <c r="B40" s="33"/>
     </row>
     <row r="41" spans="2:2">
-      <c r="B41" s="32"/>
+      <c r="B41" s="33"/>
     </row>
     <row r="42" spans="2:2">
-      <c r="B42" s="32"/>
+      <c r="B42" s="33"/>
     </row>
     <row r="43" spans="2:2">
-      <c r="B43" s="32"/>
+      <c r="B43" s="33"/>
     </row>
     <row r="44" spans="2:2">
-      <c r="B44" s="32"/>
+      <c r="B44" s="33"/>
     </row>
     <row r="45" spans="2:2">
-      <c r="B45" s="32"/>
+      <c r="B45" s="33"/>
     </row>
     <row r="46" spans="2:2">
-      <c r="B46" s="32"/>
+      <c r="B46" s="33"/>
     </row>
-    <row r="47" spans="2:2">
-      <c r="B47" s="32"/>
-    </row>
-    <row r="51" spans="7:7">
-      <c r="G51" s="35"/>
+    <row r="50" spans="7:7">
+      <c r="G50" s="36"/>
     </row>
   </sheetData>
-  <mergeCells count="6">
-    <mergeCell ref="J14:N14"/>
+  <mergeCells count="5">
+    <mergeCell ref="J13:N13"/>
     <mergeCell ref="G5:M5"/>
     <mergeCell ref="A6:N6"/>
     <mergeCell ref="A8:N8"/>
-    <mergeCell ref="J13:N13"/>
-    <mergeCell ref="L12:N12"/>
+    <mergeCell ref="J12:N12"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="7.874015748031496E-2" right="7.874015748031496E-2" top="7.874015748031496E-2" bottom="7.874015748031496E-2" header="0.19685039370078741" footer="0.19685039370078741"/>
   <pageSetup paperSize="9" scale="80" orientation="landscape" verticalDpi="300" r:id="rId1"/>
-  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>